<commit_message>
Doc Fabricacion actualizada para SETI (Nov-22)
Fabricacion de primer prototipo en SETI (4 juegos)
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CONNECTOR.xlsx
+++ b/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CONNECTOR.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER-1K\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5958562-3C2F-4011-B36D-B708EAF41D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336BD717-A4E1-B946-B270-6C7A93A786F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CONNECTOR" sheetId="1" r:id="rId1"/>
+    <sheet name="_HISTORY" sheetId="2" r:id="rId2"/>
+    <sheet name="CONTACT INFO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Qty</t>
   </si>
@@ -86,13 +88,76 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Transil</t>
+  </si>
+  <si>
+    <t>HISTORY</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>autor</t>
+  </si>
+  <si>
+    <t>cambios</t>
+  </si>
+  <si>
+    <t>DGB</t>
+  </si>
+  <si>
+    <t>Añadida descripcion de componentes y numero de posicion</t>
+  </si>
+  <si>
+    <t>Document property of:</t>
+  </si>
+  <si>
+    <t>EXINOM CORE SL</t>
+  </si>
+  <si>
+    <t>Calle Aranjuez, 513</t>
+  </si>
+  <si>
+    <t>Alcala de Henares</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>david@exinom.com</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +34 603486681</t>
+  </si>
+  <si>
+    <t>JRC</t>
+  </si>
+  <si>
+    <t>Creacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +328,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,8 +581,14 @@
         <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -643,6 +768,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -689,7 +823,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -715,6 +849,7 @@
     <xf numFmtId="0" fontId="21" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -724,79 +859,74 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -846,6 +976,31 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
@@ -862,7 +1017,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H10" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H10" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A6:H10" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H10">
     <sortCondition ref="D6:D10"/>
@@ -882,7 +1037,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1181,52 +1336,52 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="146" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -1252,7 +1407,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1266,16 +1424,19 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1289,16 +1450,19 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>3</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1312,12 +1476,12 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="11" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1326,13 +1490,13 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B9">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1346,4 +1510,155 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F394E835-0523-104C-AA22-72C38CD42C08}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15">
+        <v>44874</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15">
+        <v>44880</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7484491A-13D6-E342-9FF7-B451D2DA0066}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>28805</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" display="mailto:david@exinom.com" xr:uid="{52A1AECB-2168-D643-A872-157F6C593DCE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
BOM PCB Connector Actualizada y SCH
Se actualiza la BOM con el nuevo transistor Q1 DMG3415U-7
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CONNECTOR.xlsx
+++ b/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CONNECTOR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336BD717-A4E1-B946-B270-6C7A93A786F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F163DF9-6776-BB40-B196-6E4AE949BF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,25 @@
     <sheet name="_HISTORY" sheetId="2" r:id="rId2"/>
     <sheet name="CONTACT INFO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Qty</t>
   </si>
@@ -54,27 +67,15 @@
     <t>Link</t>
   </si>
   <si>
-    <t>PJA3416AE_R1_00001</t>
-  </si>
-  <si>
     <t>S1761-42R</t>
   </si>
   <si>
     <t>SM2T18A</t>
   </si>
   <si>
-    <t>SOT23_PJA3416_PNJ</t>
-  </si>
-  <si>
-    <t>S176142R</t>
-  </si>
-  <si>
     <t>H1, H2</t>
   </si>
   <si>
-    <t>https://www.digikey.es/es/products/detail/panjit-international-inc/PJA3416AE-R1-00001/14660222?s=N4IgTCBcDaIAoCkCCBmALARgGxIKIH0AlDfABnNIxAF0BfIA</t>
-  </si>
-  <si>
     <t>https://www.digikey.es/es/products/detail/harwin-inc/S1761-42R/2264460?s=N4IgTCBcDaIMoEYDsA2BBaALGASiAugL5A</t>
   </si>
   <si>
@@ -151,13 +152,34 @@
   </si>
   <si>
     <t>Creacion</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/en/products/detail/diodes-incorporated/DMG3415U-7/2052768</t>
+  </si>
+  <si>
+    <t>DMG3415U-7</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t>DO-216AA</t>
+  </si>
+  <si>
+    <t>5-ENE-23</t>
+  </si>
+  <si>
+    <t>Se cambia Q1. Actualizado package de D1</t>
+  </si>
+  <si>
+    <t>VERSION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,8 +404,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -584,6 +613,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,36 +870,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -875,11 +903,24 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -927,6 +968,31 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -976,31 +1042,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
@@ -1017,7 +1058,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H10" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H10" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A6:H10" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H10">
     <sortCondition ref="D6:D10"/>
@@ -1335,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1353,57 +1394,61 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="22">
+        <f>MAX(_HISTORY!A4:A42)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1412,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1421,16 +1466,16 @@
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1438,25 +1483,22 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1464,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1473,16 +1515,16 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>18</v>
+        <v>42</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1490,34 +1532,33 @@
     <mergeCell ref="B4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B9">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H7" r:id="rId1" xr:uid="{B7721278-4E8C-4E3E-9385-67AADD5EEA10}"/>
-    <hyperlink ref="H8" r:id="rId2" xr:uid="{435480B1-CE15-4999-8D8F-00BEE347DD1F}"/>
-    <hyperlink ref="H9" r:id="rId3" xr:uid="{6703EE6D-776C-4569-A59F-0F4859E42F44}"/>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{435480B1-CE15-4999-8D8F-00BEE347DD1F}"/>
+    <hyperlink ref="H9" r:id="rId2" xr:uid="{6703EE6D-776C-4569-A59F-0F4859E42F44}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F394E835-0523-104C-AA22-72C38CD42C08}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1526,50 +1567,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="10">
         <v>44874</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="10">
         <v>44880</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1589,68 +1644,68 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+    </row>
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="11">
+        <v>28805</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+    </row>
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-    </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
-        <v>28805</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="B9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="19"/>
-    </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
BOM actualizadas para fabricacion 1ra SETI
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CONNECTOR.xlsx
+++ b/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CONNECTOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F163DF9-6776-BB40-B196-6E4AE949BF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86021842-7470-234A-9076-3FA13901FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1377,7 +1377,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>